<commit_message>
Descripción de los cambios
</commit_message>
<xml_diff>
--- a/Asistencia_concurso de escoltas_2025-02-15.xlsx
+++ b/Asistencia_concurso de escoltas_2025-02-15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Firma</t>
+          <t>Firma.1</t>
         </is>
       </c>
     </row>
@@ -486,6 +486,28 @@
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ALBARRAN  JIMENEZ OSCAR EDUARDO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23:42:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>23:42:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>